<commit_message>
Chore: changed kinetics column names to use plural
To be compatible with kineticsDB
</commit_message>
<xml_diff>
--- a/examples/example_files/model_v2.3.xlsx
+++ b/examples/example_files/model_v2.3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -775,10 +775,10 @@
     <t>activators</t>
   </si>
   <si>
-    <t>negative effector</t>
-  </si>
-  <si>
-    <t>positive effector</t>
+    <t>negative effectors</t>
+  </si>
+  <si>
+    <t>positive effectors</t>
   </si>
   <si>
     <t>allosteric</t>
@@ -787,40 +787,40 @@
     <t>subunits</t>
   </si>
   <si>
-    <t>mechanism_ref_type</t>
-  </si>
-  <si>
-    <t>mechanism_ref</t>
-  </si>
-  <si>
-    <t>inhibitors_ref_type</t>
-  </si>
-  <si>
-    <t>inhibitors_ref</t>
-  </si>
-  <si>
-    <t>activators_ref_type</t>
-  </si>
-  <si>
-    <t>activators_ref</t>
-  </si>
-  <si>
-    <t>negative_effectors_ref_type</t>
-  </si>
-  <si>
-    <t>negative_effectors_ref</t>
-  </si>
-  <si>
-    <t>positive_effectors_ref_type</t>
-  </si>
-  <si>
-    <t>positive_effectors_ref</t>
-  </si>
-  <si>
-    <t>subunits_ref_type</t>
-  </si>
-  <si>
-    <t>subunits_ref</t>
+    <t>mechanism_refs_type</t>
+  </si>
+  <si>
+    <t>mechanism_refs</t>
+  </si>
+  <si>
+    <t>inhibitors_refs_type</t>
+  </si>
+  <si>
+    <t>inhibitors_refs</t>
+  </si>
+  <si>
+    <t>activators_refs_type</t>
+  </si>
+  <si>
+    <t>activators_refs</t>
+  </si>
+  <si>
+    <t>negative_effectors_refs_type</t>
+  </si>
+  <si>
+    <t>negative_effectors_refs</t>
+  </si>
+  <si>
+    <t>positive_effectors_refs_type</t>
+  </si>
+  <si>
+    <t>positive_effectors_refs</t>
+  </si>
+  <si>
+    <t>subunits_refs_type</t>
+  </si>
+  <si>
+    <t>subunits_refs</t>
   </si>
   <si>
     <t>comments</t>
@@ -1121,7 +1121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1147,6 +1147,14 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1209,11 +1217,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1222,7 +1230,15 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1247,7 +1263,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1377,7 +1393,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2254,7 +2270,7 @@
   <dimension ref="A1:D50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2981,7 +2997,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3735,8 +3751,8 @@
   </sheetPr>
   <dimension ref="A1:X50"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3744,41 +3760,41 @@
     <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>251</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -4387,7 +4403,7 @@
       <c r="V19" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="W19" s="2" t="s">
+      <c r="W19" s="4" t="s">
         <v>311</v>
       </c>
     </row>
@@ -4445,7 +4461,7 @@
       <c r="V21" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="W21" s="2" t="s">
+      <c r="W21" s="4" t="s">
         <v>317</v>
       </c>
     </row>
@@ -4477,7 +4493,7 @@
       <c r="V22" s="0" t="s">
         <v>316</v>
       </c>
-      <c r="W22" s="2" t="s">
+      <c r="W22" s="4" t="s">
         <v>317</v>
       </c>
     </row>
@@ -4602,7 +4618,7 @@
       <c r="V26" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="W26" s="2" t="s">
+      <c r="W26" s="4" t="s">
         <v>328</v>
       </c>
     </row>
@@ -4628,7 +4644,7 @@
       <c r="V27" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="W27" s="2" t="s">
+      <c r="W27" s="4" t="s">
         <v>331</v>
       </c>
     </row>
@@ -5136,7 +5152,7 @@
   <dimension ref="A1:AZ50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13063,7 +13079,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13974,7 +13990,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14704,7 +14720,7 @@
   <dimension ref="A2:A51"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14981,7 +14997,7 @@
   <dimension ref="A2:A53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15268,7 +15284,7 @@
   <dimension ref="A2:A53"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15554,8 +15570,8 @@
   </sheetPr>
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J39" activeCellId="1" sqref="1:1 J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16149,7 +16165,7 @@
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Chore: removed build ode file from example notebook
</commit_message>
<xml_diff>
--- a/examples/example_files/model_v2.3.xlsx
+++ b/examples/example_files/model_v2.3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="358">
   <si>
     <t xml:space="preserve">General Reaction and Sampling Platform (GRASP)</t>
   </si>
@@ -731,6 +731,12 @@
   </si>
   <si>
     <t xml:space="preserve">vref_std (mmol/L/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_mean2 (mmol/L/h)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vref_std2 (mmol/L/h)</t>
   </si>
   <si>
     <t xml:space="preserve">reaction/enzyme ID</t>
@@ -1364,8 +1370,8 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1384,10 +1390,10 @@
         <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2252,16 +2258,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2982,13 +2988,13 @@
         <v>118</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3737,73 +3743,73 @@
         <v>175</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3811,7 +3817,7 @@
         <v>69</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J2" s="0" t="n">
         <v>0</v>
@@ -3820,10 +3826,10 @@
         <v>1</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3831,25 +3837,25 @@
         <v>70</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="J3" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>261</v>
-      </c>
       <c r="M3" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3857,13 +3863,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -3872,10 +3878,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3883,7 +3889,7 @@
         <v>72</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>26</v>
@@ -3903,13 +3909,13 @@
         <v>73</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="H6" s="0" t="s">
         <v>57</v>
@@ -3921,13 +3927,13 @@
         <v>2</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="S6" s="0" t="n">
         <v>5470828</v>
@@ -3938,7 +3944,7 @@
         <v>74</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>29</v>
@@ -3958,13 +3964,13 @@
         <v>75</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="J8" s="0" t="n">
         <v>0</v>
@@ -3978,16 +3984,16 @@
         <v>76</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="J9" s="0" t="n">
         <v>0</v>
@@ -4001,16 +4007,16 @@
         <v>77</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="J10" s="0" t="n">
         <v>0</v>
@@ -4024,13 +4030,13 @@
         <v>78</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>0</v>
@@ -4039,16 +4045,16 @@
         <v>1</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4056,13 +4062,13 @@
         <v>79</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>0</v>
@@ -4076,16 +4082,16 @@
         <v>80</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="I13" s="0" t="s">
         <v>25</v>
@@ -4097,31 +4103,31 @@
         <v>2</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="U13" s="0" t="n">
         <v>6815421</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>6815421</v>
@@ -4132,19 +4138,19 @@
         <v>81</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I14" s="0" t="s">
         <v>25</v>
@@ -4156,31 +4162,31 @@
         <v>2</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="U14" s="0" t="n">
         <v>6815421</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>6815421</v>
@@ -4191,19 +4197,19 @@
         <v>82</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="I15" s="0" t="s">
         <v>25</v>
@@ -4215,31 +4221,31 @@
         <v>2</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="U15" s="0" t="n">
         <v>6815421</v>
       </c>
       <c r="V15" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>6815421</v>
@@ -4250,7 +4256,7 @@
         <v>83</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>38</v>
@@ -4270,16 +4276,16 @@
         <v>84</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="H17" s="0" t="s">
         <v>34</v>
@@ -4291,19 +4297,19 @@
         <v>2</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M17" s="0" t="n">
         <v>19686854</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="O17" s="0" t="n">
         <v>4154932</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>19686854</v>
@@ -4314,16 +4320,16 @@
         <v>85</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="H18" s="0" t="s">
         <v>34</v>
@@ -4335,19 +4341,19 @@
         <v>2</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M18" s="0" t="n">
         <v>19686854</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="O18" s="0" t="n">
         <v>4154932</v>
       </c>
       <c r="V18" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W18" s="0" t="n">
         <v>19686854</v>
@@ -4358,7 +4364,7 @@
         <v>86</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>40</v>
@@ -4373,10 +4379,10 @@
         <v>2</v>
       </c>
       <c r="V19" s="0" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4384,7 +4390,7 @@
         <v>87</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>40</v>
@@ -4399,10 +4405,10 @@
         <v>2</v>
       </c>
       <c r="V20" s="0" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4410,13 +4416,13 @@
         <v>88</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="J21" s="0" t="n">
         <v>0</v>
@@ -4425,16 +4431,16 @@
         <v>2</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M21" s="0" t="n">
         <v>17914867</v>
       </c>
       <c r="V21" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4442,13 +4448,13 @@
         <v>89</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="J22" s="0" t="n">
         <v>0</v>
@@ -4457,16 +4463,16 @@
         <v>2</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M22" s="0" t="n">
         <v>17914867</v>
       </c>
       <c r="V22" s="0" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4474,13 +4480,13 @@
         <v>90</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="J23" s="0" t="n">
         <v>0</v>
@@ -4489,16 +4495,16 @@
         <v>2</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M23" s="0" t="n">
         <v>8805555</v>
       </c>
       <c r="V23" s="0" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="W23" s="0" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4506,7 +4512,7 @@
         <v>91</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>28</v>
@@ -4524,13 +4530,13 @@
         <v>2</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="O24" s="0" t="n">
         <v>4154932</v>
       </c>
       <c r="V24" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W24" s="0" t="n">
         <v>6326623</v>
@@ -4541,13 +4547,13 @@
         <v>92</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>47</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="J25" s="0" t="n">
         <v>0</v>
@@ -4556,13 +4562,13 @@
         <v>3</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="V25" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W25" s="0" t="n">
         <v>12876349</v>
@@ -4573,7 +4579,7 @@
         <v>93</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>25</v>
@@ -4588,10 +4594,10 @@
         <v>2</v>
       </c>
       <c r="V26" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4599,13 +4605,13 @@
         <v>94</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="J27" s="0" t="n">
         <v>0</v>
@@ -4614,10 +4620,10 @@
         <v>4</v>
       </c>
       <c r="V27" s="0" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4625,10 +4631,10 @@
         <v>95</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>49</v>
@@ -4640,16 +4646,16 @@
         <v>4</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="V28" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="W28" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4657,7 +4663,7 @@
         <v>96</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>43</v>
@@ -4672,10 +4678,10 @@
         <v>2</v>
       </c>
       <c r="V29" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="W29" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4683,13 +4689,13 @@
         <v>97</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="H30" s="0" t="s">
         <v>55</v>
@@ -4701,13 +4707,13 @@
         <v>4</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M30" s="0" t="n">
         <v>7447472</v>
       </c>
       <c r="V30" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W30" s="0" t="n">
         <v>8636984</v>
@@ -4718,13 +4724,13 @@
         <v>98</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="J31" s="0" t="n">
         <v>0</v>
@@ -4733,16 +4739,16 @@
         <v>1</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="M31" s="0" t="n">
         <v>5128739</v>
       </c>
       <c r="V31" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="W31" s="0" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4750,7 +4756,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>52</v>
@@ -4765,10 +4771,10 @@
         <v>1</v>
       </c>
       <c r="V32" s="0" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="W32" s="0" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4776,7 +4782,7 @@
         <v>100</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>53</v>
@@ -4791,7 +4797,7 @@
         <v>2</v>
       </c>
       <c r="V33" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W33" s="0" t="n">
         <v>9376357</v>
@@ -4802,16 +4808,16 @@
         <v>101</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="J34" s="0" t="n">
         <v>1</v>
@@ -4820,19 +4826,19 @@
         <v>4</v>
       </c>
       <c r="L34" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M34" s="0" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="T34" s="0" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="U34" s="0" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="V34" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="W34" s="0" t="n">
         <v>468836</v>
@@ -4843,10 +4849,10 @@
         <v>102</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D35" s="0" t="s">
         <v>57</v>
@@ -4858,16 +4864,16 @@
         <v>1</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="V35" s="0" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="W35" s="0" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4875,13 +4881,13 @@
         <v>103</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="J36" s="0" t="n">
         <v>0</v>
@@ -4890,16 +4896,16 @@
         <v>1</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="V36" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="W36" s="0" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4907,7 +4913,7 @@
         <v>104</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J37" s="0" t="n">
         <v>0</v>
@@ -4921,7 +4927,7 @@
         <v>105</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J38" s="0" t="n">
         <v>0</v>
@@ -4935,7 +4941,7 @@
         <v>106</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J39" s="0" t="n">
         <v>0</v>
@@ -4949,7 +4955,7 @@
         <v>107</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J40" s="0" t="n">
         <v>0</v>
@@ -4963,7 +4969,7 @@
         <v>108</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J41" s="0" t="n">
         <v>0</v>
@@ -4977,7 +4983,7 @@
         <v>109</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J42" s="0" t="n">
         <v>0</v>
@@ -4991,7 +4997,7 @@
         <v>110</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J43" s="0" t="n">
         <v>0</v>
@@ -5005,7 +5011,7 @@
         <v>111</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J44" s="0" t="n">
         <v>0</v>
@@ -5019,7 +5025,7 @@
         <v>112</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J45" s="0" t="n">
         <v>0</v>
@@ -5033,7 +5039,7 @@
         <v>113</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J46" s="0" t="n">
         <v>0</v>
@@ -5047,7 +5053,7 @@
         <v>114</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J47" s="0" t="n">
         <v>0</v>
@@ -5061,7 +5067,7 @@
         <v>115</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J48" s="0" t="n">
         <v>0</v>
@@ -5075,7 +5081,7 @@
         <v>116</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J49" s="0" t="n">
         <v>0</v>
@@ -5089,7 +5095,7 @@
         <v>117</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J50" s="0" t="n">
         <v>0</v>
@@ -16293,7 +16299,7 @@
   </sheetPr>
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>